<commit_message>
Changes in Excel done
</commit_message>
<xml_diff>
--- a/Leads And Coordinator/controller/Techy Ludo attendees.xlsx
+++ b/Leads And Coordinator/controller/Techy Ludo attendees.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -20,6 +20,9 @@
   </si>
   <si>
     <t>College</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
   </si>
   <si>
     <t>Purchase_Type</t>
@@ -37,6 +40,9 @@
     <t>GCET</t>
   </si>
   <si>
+    <t>7016763640</t>
+  </si>
+  <si>
     <t>EVENT</t>
   </si>
   <si>
@@ -47,6 +53,9 @@
   </si>
   <si>
     <t>prathamshah019@gmail.com</t>
+  </si>
+  <si>
+    <t>7405802474</t>
   </si>
 </sst>
 </file>
@@ -92,13 +101,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -114,39 +123,48 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="0" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="0" t="s">
+      <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="F2" s="0" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>13</v>
+      </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in lead controller
</commit_message>
<xml_diff>
--- a/Leads And Coordinator/controller/Techy Ludo attendees.xlsx
+++ b/Leads And Coordinator/controller/Techy Ludo attendees.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -19,36 +19,36 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Enrollment</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
     <t>College</t>
   </si>
   <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Purchase_Type</t>
-  </si>
-  <si>
-    <t>Payment_Mode</t>
-  </si>
-  <si>
     <t>Kandarp Shah</t>
   </si>
   <si>
     <t>shahkandarp24@gmail.com</t>
   </si>
   <si>
+    <t>7016763640</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
     <t>GCET</t>
   </si>
   <si>
-    <t>7016763640</t>
-  </si>
-  <si>
-    <t>EVENT</t>
-  </si>
-  <si>
-    <t>OFFLINE</t>
-  </si>
-  <si>
     <t>Pratham Shah</t>
   </si>
   <si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>7405802474</t>
+  </si>
+  <si>
+    <t>Het Patel</t>
+  </si>
+  <si>
+    <t>hetpatel5542@gmail.com</t>
+  </si>
+  <si>
+    <t>7698545581</t>
   </si>
 </sst>
 </file>
@@ -101,13 +110,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -126,28 +135,34 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:7">
       <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
@@ -155,15 +170,41 @@
         <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="0" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>